<commit_message>
I'm so behind on pushing things
</commit_message>
<xml_diff>
--- a/ch_PFMC/Species_and_stock_assessments.xlsx
+++ b/ch_PFMC/Species_and_stock_assessments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\provo\Documents\GitHub\popdy\ch_PFMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D4BEB1-C74D-4ED3-BD0A-45165D9DB0EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1ED9AB-FF7B-47C4-A3F6-9A8D83039F1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21360" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,8 @@
     <sheet name="Stock_assessments" sheetId="1" r:id="rId1"/>
     <sheet name="Life_history_table" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="maturity_coefficients" sheetId="4" r:id="rId4"/>
+    <sheet name="selectivity_coefficients" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="159">
   <si>
     <t>species_name</t>
   </si>
@@ -491,6 +493,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>slope,intercept</t>
+  </si>
+  <si>
+    <t>pg_in_stockass</t>
+  </si>
+  <si>
+    <t>https://www.pcouncil.org/wp-content/uploads/2019/02/2018_HMS_SAFE_Report_archive_copy.pdf</t>
+  </si>
+  <si>
+    <t>2015 (2018)</t>
+  </si>
+  <si>
+    <t>2015 (2017)</t>
+  </si>
+  <si>
+    <t>https://www.pcouncil.org/wp-content/uploads/2018/02/FINAL_2017_Bocaccio_Update_Assessment_February_2_2018.pdf</t>
   </si>
 </sst>
 </file>
@@ -610,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -675,12 +695,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -698,6 +712,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1015,1114 +1036,1114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD8"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="28"/>
-    <col min="2" max="2" width="16.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="28" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="17" width="9.140625" style="28"/>
-    <col min="18" max="18" width="11.85546875" style="28" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="9.140625" style="26"/>
+    <col min="2" max="2" width="16.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="17" width="9.140625" style="26"/>
+    <col min="18" max="18" width="11.85546875" style="26" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="P1" s="29" t="s">
+      <c r="P1" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="27" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="A2" s="26">
         <v>2</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="26">
         <v>2015</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="29">
         <v>1</v>
       </c>
-      <c r="I2" s="34">
+      <c r="I2" s="32">
         <v>1.5</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="29">
         <v>15</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="29">
         <v>0.4</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="29">
         <v>0.81</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="29">
         <v>1981</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="29">
         <v>2008</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="29">
         <v>0.5</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="P2" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q2" s="31">
+      <c r="Q2" s="29">
         <v>2.25</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="28">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E3" s="26">
         <v>2014</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="29">
         <v>1.5</v>
       </c>
-      <c r="I3" s="34">
+      <c r="I3" s="32">
         <v>1.5</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="29">
         <v>14</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="29">
         <v>0.5</v>
       </c>
-      <c r="L3" s="31">
+      <c r="L3" s="29">
         <v>1</v>
       </c>
-      <c r="M3" s="31">
+      <c r="M3" s="29">
         <v>1962</v>
       </c>
-      <c r="N3" s="31">
+      <c r="N3" s="29">
         <v>2008</v>
       </c>
-      <c r="O3" s="31">
+      <c r="O3" s="29">
         <v>0.32400000000000001</v>
       </c>
-      <c r="P3" s="31" t="s">
+      <c r="P3" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="29">
         <v>0.47</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="28">
+      <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="28">
-        <v>2015</v>
-      </c>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="31">
+      <c r="G4" s="35" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="29">
         <v>2.5</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="29">
         <v>1</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="29">
         <v>7</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="29">
         <v>0.6</v>
       </c>
-      <c r="M4" s="31">
+      <c r="M4" s="29">
         <v>1975</v>
       </c>
-      <c r="N4" s="31">
+      <c r="N4" s="29">
         <v>2007</v>
       </c>
-      <c r="O4" s="31">
+      <c r="O4" s="29">
         <v>0.76</v>
       </c>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q4" s="31">
+      <c r="Q4" s="29">
         <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="28">
+      <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E5" s="28">
-        <v>2015</v>
-      </c>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F5" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="29">
         <v>4</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="29">
         <v>1</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="29">
         <v>12</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="29">
         <v>0.6</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="29">
         <v>1975</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="29">
         <v>2007</v>
       </c>
-      <c r="O5" s="31"/>
-      <c r="P5" s="31" t="s">
+      <c r="O5" s="29"/>
+      <c r="P5" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="28">
+      <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="28">
-        <v>2016</v>
-      </c>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="29">
         <v>4</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="29">
         <v>3</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="29">
         <v>26</v>
       </c>
-      <c r="K6" s="31" t="s">
+      <c r="K6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="29">
         <v>0.6</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="29">
         <v>1951</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="29">
         <v>2007</v>
       </c>
-      <c r="O6" s="31">
+      <c r="O6" s="29">
         <v>0.19500000000000001</v>
       </c>
-      <c r="P6" s="31" t="s">
+      <c r="P6" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q6" s="31">
+      <c r="Q6" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="28">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="26">
         <v>2015</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="29">
         <v>3</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="29">
         <v>3</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="29">
         <v>4</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="29">
         <v>0.16250000000000001</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="29">
         <v>0.1</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="29">
         <v>1970</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="29">
         <v>2010</v>
       </c>
-      <c r="O7" s="31"/>
-      <c r="P7" s="31" t="s">
+      <c r="O7" s="29"/>
+      <c r="P7" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q7" s="31">
+      <c r="Q7" s="29">
         <v>0.94</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="28">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="26">
         <v>2015</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="32" t="s">
+      <c r="I8" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="J8" s="32" t="s">
+      <c r="J8" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="29">
         <v>0.17</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="29">
         <v>0.1</v>
       </c>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
-      <c r="O8" s="31"/>
-      <c r="P8" s="31" t="s">
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="29">
         <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="28">
-        <v>2015</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="29">
         <v>3</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="29">
         <v>3</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="29">
         <v>40</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="29">
         <v>0.15</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="29">
         <v>1</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="29">
         <v>1970</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="29">
         <v>2008</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="29">
         <v>0.22</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q9" s="31">
+      <c r="Q9" s="29">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="28">
+      <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E10" s="26">
         <v>2009</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="31">
+      <c r="G10" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="H10" s="29">
         <v>3</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="29">
         <v>3</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="29">
         <v>13</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="29">
         <v>0.25</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="29">
         <v>0.7</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="29">
         <v>1970</v>
       </c>
-      <c r="N10" s="31">
+      <c r="N10" s="29">
         <v>2006</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="29">
         <v>0.16</v>
       </c>
-      <c r="P10" s="31" t="s">
+      <c r="P10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q10" s="31">
+      <c r="Q10" s="29">
         <v>0.7</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="26">
         <v>2015</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="30" t="s">
+      <c r="G11" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="29">
         <v>10</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="29">
         <v>10</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="29">
         <v>95</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="29">
         <v>0.06</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="29">
         <v>0.5</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="29">
         <v>1960</v>
       </c>
-      <c r="N11" s="31">
+      <c r="N11" s="29">
         <v>2009</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="29">
         <v>0.13</v>
       </c>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="Q11" s="31">
+      <c r="Q11" s="29">
         <v>0.51</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="28">
+      <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E12" s="26">
         <v>2015</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="30" t="s">
+      <c r="G12" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="29">
         <v>3</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="29">
         <v>5</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="29">
         <v>35</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="29">
         <v>0.16</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="29">
         <v>1</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="29">
         <v>1965</v>
       </c>
-      <c r="N12" s="31">
+      <c r="N12" s="29">
         <v>2009</v>
       </c>
-      <c r="O12" s="31">
+      <c r="O12" s="29">
         <v>0.25</v>
       </c>
-      <c r="P12" s="31" t="s">
+      <c r="P12" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q12" s="31">
+      <c r="Q12" s="29">
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="28">
+      <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E13" s="26">
         <v>2015</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="29">
         <v>7</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="29">
         <v>6</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="29">
         <v>105</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="29">
         <v>0.8</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="29">
         <v>1975</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="29">
         <v>2007</v>
       </c>
-      <c r="O13" s="31">
+      <c r="O13" s="29">
         <v>0.2</v>
       </c>
-      <c r="P13" s="31" t="s">
+      <c r="P13" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q13" s="31">
+      <c r="Q13" s="29">
         <v>0.95</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="28">
+      <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E14" s="26">
         <v>2011</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31">
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29">
         <v>0.09</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="29">
         <v>0.35</v>
       </c>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31" t="s">
+      <c r="M14" s="29"/>
+      <c r="N14" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="29">
         <v>0.11899999999999999</v>
       </c>
-      <c r="P14" s="31" t="s">
+      <c r="P14" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q14" s="31">
+      <c r="Q14" s="29">
         <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="28">
+      <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="26" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="26">
         <v>2007</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="29">
         <v>3</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="29">
         <v>5</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="29">
         <v>22</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="29">
         <v>0.26</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="29">
         <v>0.42</v>
       </c>
-      <c r="M15" s="31">
+      <c r="M15" s="29">
         <v>1940</v>
       </c>
-      <c r="N15" s="31">
+      <c r="N15" s="29">
         <v>2006</v>
       </c>
-      <c r="O15" s="31">
+      <c r="O15" s="29">
         <v>0.3</v>
       </c>
-      <c r="P15" s="31" t="s">
+      <c r="P15" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q15" s="31">
+      <c r="Q15" s="29">
         <v>0.83</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="28">
+      <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="28">
+      <c r="E16" s="26">
         <v>2009</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="29">
         <v>5</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="29">
         <v>3</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="29">
         <v>18</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="29">
         <v>0.18</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="29">
         <v>0.5</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="29">
         <v>1930</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="29">
         <v>2008</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="29">
         <v>0.13</v>
       </c>
-      <c r="P16" s="31" t="s">
+      <c r="P16" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q16" s="31">
+      <c r="Q16" s="29">
         <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="26" t="s">
         <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E17" s="28">
+      <c r="E17" s="26">
         <v>2016</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="29">
         <v>3</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="29">
         <v>4</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="29">
         <v>22</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="29">
         <v>0.23</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="29">
         <v>1.1299999999999999</v>
       </c>
-      <c r="M17" s="31">
+      <c r="M17" s="29">
         <v>1960</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="29">
         <v>2008</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="29">
         <v>0.3</v>
       </c>
-      <c r="P17" s="31" t="s">
+      <c r="P17" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Q17" s="31">
+      <c r="Q17" s="29">
         <v>0.88</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="28">
+      <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="26" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="26">
         <v>2011</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="30" t="s">
+      <c r="G18" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="29">
         <v>8</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="29">
         <v>8</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="29">
         <v>100</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="29">
         <v>0.05</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="29">
         <v>1</v>
       </c>
-      <c r="M18" s="31">
+      <c r="M18" s="29">
         <v>1956</v>
       </c>
-      <c r="N18" s="31">
+      <c r="N18" s="29">
         <v>2007</v>
       </c>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31" t="s">
+      <c r="O18" s="29"/>
+      <c r="P18" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q18" s="31">
+      <c r="Q18" s="29">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="28">
+      <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="26" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E19" s="28">
+      <c r="E19" s="26">
         <v>2014</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G19" s="30" t="s">
+      <c r="G19" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="29">
         <v>6</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="29">
         <v>6</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="29">
         <v>31</v>
       </c>
-      <c r="K19" s="31">
+      <c r="K19" s="29">
         <v>0.15</v>
       </c>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31">
+      <c r="L19" s="29"/>
+      <c r="M19" s="29">
         <v>1939</v>
       </c>
-      <c r="N19" s="31">
+      <c r="N19" s="29">
         <v>2008</v>
       </c>
-      <c r="O19" s="31">
+      <c r="O19" s="29">
         <v>0.16</v>
       </c>
-      <c r="P19" s="31" t="s">
+      <c r="P19" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q19" s="31">
+      <c r="Q19" s="29">
         <v>0.95</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="26" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="26">
         <v>2015</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G20" s="30" t="s">
+      <c r="G20" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="29">
         <v>3</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="29">
         <v>3</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="29">
         <v>85</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="29">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="29">
         <v>0.6</v>
       </c>
-      <c r="M20" s="31">
+      <c r="M20" s="29">
         <v>1971</v>
       </c>
-      <c r="N20" s="31">
+      <c r="N20" s="29">
         <v>2006</v>
       </c>
-      <c r="O20" s="31">
+      <c r="O20" s="29">
         <v>0.246</v>
       </c>
-      <c r="P20" s="31" t="s">
+      <c r="P20" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="Q20" s="31">
+      <c r="Q20" s="29">
         <v>0.34</v>
       </c>
     </row>
     <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28">
+      <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="26" t="s">
         <v>60</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="28">
+      <c r="E21" s="26">
         <v>2015</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="G21" s="30" t="s">
+      <c r="G21" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="H21" s="33">
+      <c r="H21" s="31">
         <v>6</v>
       </c>
-      <c r="I21" s="33">
+      <c r="I21" s="31">
         <v>6</v>
       </c>
-      <c r="J21" s="33">
+      <c r="J21" s="31">
         <v>60</v>
       </c>
-      <c r="K21" s="33">
+      <c r="K21" s="31">
         <v>0.125</v>
       </c>
-      <c r="L21" s="33">
+      <c r="L21" s="31">
         <v>0.6</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="31">
         <v>1958</v>
       </c>
-      <c r="N21" s="33">
+      <c r="N21" s="31">
         <v>2008</v>
       </c>
-      <c r="O21" s="33">
+      <c r="O21" s="31">
         <v>0.17</v>
       </c>
-      <c r="P21" s="33" t="s">
+      <c r="P21" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="Q21" s="33">
+      <c r="Q21" s="31">
         <v>0.41</v>
       </c>
     </row>
@@ -2135,29 +2156,29 @@
     <hyperlink ref="F4" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="F6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G5" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G6" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G8" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F7" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F8" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="G9" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F9" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G12" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G13" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="G14" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G15" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G16" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G17" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G18" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F10:F18" r:id="rId26" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="G19" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="G20" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="G21" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F19:F21" r:id="rId30" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F7" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F8" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F9" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G14" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G15" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G16" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G17" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G18" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F10:F18" r:id="rId23" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G19" r:id="rId24" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G20" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G21" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F19:F21" r:id="rId27" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G4" r:id="rId28" xr:uid="{8BD314DF-77BC-41B6-AFB9-DAF515D4ECE0}"/>
+    <hyperlink ref="G10" r:id="rId29" xr:uid="{A8D84BA4-B186-492E-8DCC-E8C102DC8FE5}"/>
+    <hyperlink ref="G9" r:id="rId30" xr:uid="{12E98B0B-3238-437B-8C0D-0796F4C07FDF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId31"/>
@@ -2170,7 +2191,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2209,41 +2230,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="15"/>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
     </row>
     <row r="2" spans="1:32" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -3116,6 +3137,12 @@
       <c r="N17" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="S17" s="8">
+        <v>21</v>
+      </c>
+      <c r="T17" s="8">
+        <v>140</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
@@ -3489,7 +3516,7 @@
   <dimension ref="A1:AF25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:K23"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3528,41 +3555,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="15"/>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
-      <c r="AF1" s="27"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
+      <c r="AA1" s="34"/>
+      <c r="AB1" s="34"/>
+      <c r="AC1" s="34"/>
+      <c r="AD1" s="34"/>
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
     </row>
     <row r="2" spans="1:32" ht="36.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -4684,31 +4711,31 @@
     </row>
     <row r="24" spans="1:32" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="G25" s="29" t="s">
+      <c r="G25" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="I25" s="29" t="s">
+      <c r="I25" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="J25" s="29" t="s">
+      <c r="J25" s="27" t="s">
         <v>147</v>
       </c>
-      <c r="K25" s="29" t="s">
+      <c r="K25" s="27" t="s">
         <v>148</v>
       </c>
       <c r="L25" s="8"/>
@@ -4720,4 +4747,625 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7E5121-224A-4679-9A10-26615325339B}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="26"/>
+    <col min="2" max="2" width="16.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="26" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="26" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>2</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="26">
+        <v>2014</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="29">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>3</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>4</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>5</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="26">
+        <v>2016</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="26">
+        <v>2009</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
+        <v>11</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <v>12</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
+        <v>13</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="26">
+        <v>2011</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="29"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
+        <v>14</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="26">
+        <v>2007</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>15</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="26">
+        <v>2009</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" s="29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
+        <v>16</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" s="26">
+        <v>2016</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
+        <v>17</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="26">
+        <v>2011</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
+        <v>18</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E19" s="26">
+        <v>2014</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E20" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="26">
+        <v>20</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="26">
+        <v>2015</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="31">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{3F4A7757-12F2-4E27-B581-4EF200107502}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{4479EF44-98A1-436A-8F3B-B5DDD75F3593}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{CEA5E980-6E7F-433F-B5C6-4F11C3A381E8}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{E7A7DA28-D7B3-4246-A6E3-17A46DB0B453}"/>
+    <hyperlink ref="F4" r:id="rId5" xr:uid="{5E2F3536-B320-4FF0-8777-020AD6D08E72}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{4E773E3D-6C34-4A7C-99CC-1DF514BFADD4}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{1FC3A80E-3385-4BD0-9D44-5023A6C88C93}"/>
+    <hyperlink ref="G4" r:id="rId8" xr:uid="{953E894B-C45B-46FA-BBC6-D40ACE21ED39}"/>
+    <hyperlink ref="G5" r:id="rId9" xr:uid="{10994061-1221-4963-A93F-582CFD7F9D59}"/>
+    <hyperlink ref="G6" r:id="rId10" xr:uid="{3C9FB49C-25D6-4AAB-843A-188EEED480F9}"/>
+    <hyperlink ref="G7" r:id="rId11" xr:uid="{561380BF-A427-42AA-979E-FC63839D2A49}"/>
+    <hyperlink ref="G8" r:id="rId12" xr:uid="{973E0AC8-6519-4E8A-A82D-62531150C749}"/>
+    <hyperlink ref="F7" r:id="rId13" xr:uid="{E9570FE0-FDB7-451C-AB4B-B5D5985AEED9}"/>
+    <hyperlink ref="F8" r:id="rId14" xr:uid="{C012C2A1-3F84-4D77-94A1-11129F70CA24}"/>
+    <hyperlink ref="G9" r:id="rId15" xr:uid="{68EABCD5-D30F-429C-917B-B68F9C430983}"/>
+    <hyperlink ref="F9" r:id="rId16" xr:uid="{6CC3E196-53F8-43DC-B53E-159CD8D670E0}"/>
+    <hyperlink ref="G10" r:id="rId17" xr:uid="{BD2384B1-9959-4444-9663-5F3236D97448}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{DFED2063-49FB-4070-B3D2-5DBD4CE14B40}"/>
+    <hyperlink ref="G12" r:id="rId19" xr:uid="{91FFE934-A0A5-4AE7-AE48-683E3AF46B96}"/>
+    <hyperlink ref="G13" r:id="rId20" xr:uid="{127063E7-D318-4030-A5F7-3EEF33D5016F}"/>
+    <hyperlink ref="G14" r:id="rId21" xr:uid="{209AB67C-3E1D-44B3-BBE4-57A58AEB6A9D}"/>
+    <hyperlink ref="G15" r:id="rId22" xr:uid="{C5F0F3D8-EEAE-42EF-ADFF-7383AC2E00C9}"/>
+    <hyperlink ref="G16" r:id="rId23" xr:uid="{EC9D1611-EFAA-42A8-AD48-961353D0A050}"/>
+    <hyperlink ref="G17" r:id="rId24" xr:uid="{2E634F02-3D00-4724-81D9-87E90E05B847}"/>
+    <hyperlink ref="G18" r:id="rId25" xr:uid="{33228F5E-788F-4116-A9CC-6A8C0E2D7530}"/>
+    <hyperlink ref="F10:F18" r:id="rId26" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{57D0C1B5-8369-4EC1-B5CB-7578AB1BCA5F}"/>
+    <hyperlink ref="G19" r:id="rId27" xr:uid="{E5623CAA-018B-4386-9644-E899B309247A}"/>
+    <hyperlink ref="G20" r:id="rId28" xr:uid="{841D4372-01C1-498A-936C-4A36A8C4ADC3}"/>
+    <hyperlink ref="G21" r:id="rId29" xr:uid="{2F0E6F42-36D9-4A37-B830-9E010847F7D0}"/>
+    <hyperlink ref="F19:F21" r:id="rId30" display="http://www.pcouncil.org/groundfish/stock-assessments/by-species/" xr:uid="{067D36D6-C104-411F-978D-228035B91D02}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAA7812-3BA7-4A0C-B25D-ED379087559C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>